<commit_message>
include excel insert func
</commit_message>
<xml_diff>
--- a/assets/test_data.xlsx
+++ b/assets/test_data.xlsx
@@ -432,51 +432,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="8" width="51" customWidth="1"/>
-    <col min="9" max="9" width="44.77734375" customWidth="1"/>
-    <col min="10" max="10" width="44.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="9" max="9" width="51" customWidth="1"/>
+    <col min="10" max="10" width="44.77734375" customWidth="1"/>
+    <col min="11" max="11" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8" customHeight="1" thickBot="1">
+    <row r="1" spans="1:10" ht="28.8" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1">
+        <v>15</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -484,28 +487,31 @@
         <v>17</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>30</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -513,21 +519,24 @@
         <v>18</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>